<commit_message>
Batch A and Batch E comparisons done
</commit_message>
<xml_diff>
--- a/control5.xlsx
+++ b/control5.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenzieobrien/mlc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C130CA5A-E092-F944-AADF-73425640556B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924E70F0-1359-8D4F-A3B5-D90173D2775E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="960" windowWidth="27640" windowHeight="15180" xr2:uid="{E5FDC9AF-733C-F748-A740-FAB0E2868DA2}"/>
+    <workbookView xWindow="14440" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{E5FDC9AF-733C-F748-A740-FAB0E2868DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="53">
   <si>
     <t>crunchy</t>
   </si>
@@ -108,9 +111,6 @@
     <t>mayanp000@gmail.com</t>
   </si>
   <si>
-    <t>jessica.daft1@marist.edu</t>
-  </si>
-  <si>
     <t>andrew.bauman1@marist.edu</t>
   </si>
   <si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>megan.burke@marist.edu</t>
-  </si>
-  <si>
-    <t>ryan.carmello1@marist.edu</t>
   </si>
   <si>
     <t>crunchy, chewy</t>
@@ -554,63 +551,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FD8086-8915-B14B-9E6B-6965B1CC4CAF}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
-      </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" t="s">
-        <v>54</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
@@ -630,28 +627,28 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
@@ -671,22 +668,22 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>4</v>
@@ -709,19 +706,19 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>4</v>
@@ -735,31 +732,31 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -770,7 +767,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
@@ -779,16 +776,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>3</v>
@@ -805,31 +802,31 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1">
         <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -840,7 +837,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -849,19 +846,19 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>4</v>
@@ -875,28 +872,28 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>4</v>
@@ -910,22 +907,22 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
@@ -934,30 +931,33 @@
         <v>3</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>2</v>
@@ -980,10 +980,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
@@ -992,16 +992,16 @@
         <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1012,10 +1012,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -1024,10 +1024,10 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>11</v>
@@ -1036,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1047,22 +1047,22 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>2</v>
@@ -1085,25 +1085,25 @@
         <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>4</v>
@@ -1120,63 +1120,57 @@
         <v>5</v>
       </c>
       <c r="B17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1190,25 +1184,25 @@
         <v>4</v>
       </c>
       <c r="B19" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1">
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>4</v>
@@ -1237,7 +1231,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>11</v>
@@ -1266,16 +1260,16 @@
         <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>7</v>
@@ -1292,22 +1286,22 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>2</v>
@@ -1327,25 +1321,25 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1">
         <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>3</v>
@@ -1362,31 +1356,31 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E24" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1400,25 +1394,25 @@
         <v>5</v>
       </c>
       <c r="B25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>4</v>
@@ -1432,31 +1426,31 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1470,25 +1464,25 @@
         <v>4</v>
       </c>
       <c r="B27" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>18</v>
@@ -1496,9 +1490,6 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1508,22 +1499,22 @@
         <v>5</v>
       </c>
       <c r="C28" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>4</v>
@@ -1535,71 +1526,12 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="1">
-        <v>2</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1">
-        <v>5</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="1">
-        <v>10</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:O1" xr:uid="{1EF7D4D9-7586-5F46-9184-07F3B73B7FF0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O28">
+      <sortCondition ref="F1:F28"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>